<commit_message>
-Updated table of LPC register according to changes made in CPLD code.
</commit_message>
<xml_diff>
--- a/XBlastMod register map.xlsx
+++ b/XBlastMod register map.xlsx
@@ -25,11 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17" count="17">
   <si>
     <t>Read</t>
   </si>
   <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
     <t>0x00FF</t>
   </si>
   <si>
@@ -42,28 +48,28 @@
     <t>GPI-0</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>SW2</t>
+    <t>A19 ctrl</t>
+  </si>
+  <si>
+    <t>D0_control/A19 ctrl</t>
+  </si>
+  <si>
+    <t>NOT D0_control</t>
+  </si>
+  <si>
+    <t>A15 ctrl</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>GPI = General Purpose input. Print various signal states.</t>
+  </si>
+  <si>
+    <t>Write</t>
   </si>
   <si>
     <t>A15</t>
-  </si>
-  <si>
-    <t>D0_control</t>
-  </si>
-  <si>
-    <t>A19 ctrl</t>
-  </si>
-  <si>
-    <t>A19</t>
-  </si>
-  <si>
-    <t>GPI = General Purpose input. Print various signal states.</t>
-  </si>
-  <si>
-    <t>Write</t>
   </si>
   <si>
     <t>0xF701</t>
@@ -208,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
@@ -237,13 +243,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="2" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="0">
@@ -288,8 +288,8 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0" zoomScale="80" tabSelected="1">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0" zoomScale="80" tabSelected="1">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -299,7 +299,7 @@
     <col min="3" max="3" style="1" width="17.54082" bestFit="1" customWidth="1"/>
     <col min="4" max="4" style="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" style="1" width="14.51531" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" style="1" width="15.19898" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" style="1" width="20.71304" bestFit="1" customWidth="1"/>
     <col min="8" max="8" style="1" width="20.32143" bestFit="1" customWidth="1"/>
     <col min="9" max="9" style="1" width="15.45408" bestFit="1" customWidth="1"/>
     <col min="10" max="10" style="1" width="17.69388" bestFit="1" customWidth="1"/>
@@ -350,20 +350,20 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="str">
-        <v>BNK1</v>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
         <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="str">
-        <v>BNK2</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
@@ -375,81 +375,81 @@
         <v>0</v>
       </c>
       <c r="K2" s="2" t="str">
-        <v>Chameleon ID (0xAA)</v>
+        <v>Chameleon ID (0xAA), only if external switches aren't toggled.</v>
       </c>
     </row>
     <row r="3" spans="1:1025">
       <c r="A3" s="7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1025">
       <c r="A4" s="7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="3" t="str">
         <v>Latch_en</v>
       </c>
       <c r="E4" s="3" t="str">
         <v>Kill mod</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3" t="str">
         <v>ltch D0_control</v>
       </c>
-      <c r="I4" s="10" t="str">
+      <c r="I4" s="3" t="str">
         <v>ltch A19_ctrl</v>
       </c>
-      <c r="J4" s="12" t="str">
-        <v>ltch_A19</v>
+      <c r="J4" s="8" t="str">
+        <v>ltch_A19/SW1</v>
       </c>
       <c r="K4" s="2" t="str">
         <v>Set A15 = '1' to ground it. Set D0_control = '1' to control D0. Vaue with "ltch" prefix will only be written if "Latch_en" is set in same command.</v>
       </c>
     </row>
     <row r="5" spans="1:1025">
-      <c r="A5" s="13" t="str">
+      <c r="A5" s="11" t="str">
         <v>0xF700</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>12</v>
+      <c r="B5" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="3" t="str">
@@ -470,17 +470,17 @@
       <c r="I5" s="3" t="str">
         <v>LCD-RS</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="14" t="str">
+      <c r="J5" s="10"/>
+      <c r="K5" s="12" t="str">
         <v>LCD data register</v>
       </c>
     </row>
     <row r="6" spans="1:1025">
-      <c r="A6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>2</v>
+      <c r="A6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -511,11 +511,11 @@
       </c>
     </row>
     <row r="7" spans="1:1025">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="3" t="str">
@@ -536,17 +536,17 @@
       <c r="I7" s="3" t="str">
         <v>LCD-BL0</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="15" t="str">
+      <c r="J7" s="10"/>
+      <c r="K7" s="13" t="str">
         <v>LCD backlight register. LSB is ignored.</v>
       </c>
     </row>
     <row r="8" spans="1:1025">
-      <c r="A8" s="13" t="str">
+      <c r="A8" s="11" t="str">
         <v>0xF703</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>12</v>
+      <c r="B8" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="3" t="str">
@@ -567,8 +567,8 @@
       <c r="I8" s="3" t="str">
         <v>LCD-CT0</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="15" t="str">
+      <c r="J8" s="10"/>
+      <c r="K8" s="13" t="str">
         <v>Contrast register</v>
       </c>
     </row>
@@ -577,7 +577,7 @@
         <v>0xF70E</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="str">
         <v>OS Bank ctrl</v>
@@ -585,17 +585,17 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K9" s="2" t="str">
         <v>SW* controls onboard banks. A19 controls TSOP A19.</v>
@@ -603,45 +603,45 @@
     </row>
     <row r="10" spans="1:1025">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:1025">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="str">
         <v>GPO-3</v>
@@ -655,7 +655,7 @@
       <c r="F11" s="4" t="str">
         <v>GPO-0</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="4" t="str">
@@ -672,12 +672,12 @@
       <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:1025">
-      <c r="A14" s="17" t="str">
+      <c r="A14" s="15" t="str">
         <v>Chameleon</v>
       </c>
     </row>
     <row r="15" spans="1:1025">
-      <c r="A15" s="18" t="str">
+      <c r="A15" s="16" t="str">
         <v>SmartXX</v>
       </c>
     </row>
@@ -703,8 +703,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" style="19" width="14.51531" bestFit="1" customWidth="1"/>
-    <col min="1026" max="16384" style="20"/>
+    <col min="1" max="1025" style="17" width="14.51531" bestFit="1" customWidth="1"/>
+    <col min="1026" max="16384" style="18"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -728,8 +728,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" style="21" width="14.51531" bestFit="1" customWidth="1"/>
-    <col min="1026" max="16384" style="22"/>
+    <col min="1" max="1025" style="19" width="14.51531" bestFit="1" customWidth="1"/>
+    <col min="1026" max="16384" style="20"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
update on table again.
</commit_message>
<xml_diff>
--- a/XBlastMod register map.xlsx
+++ b/XBlastMod register map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17" count="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16" count="16">
   <si>
     <t>Read</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Write</t>
-  </si>
-  <si>
-    <t>A15</t>
   </si>
   <si>
     <t>0xF701</t>
@@ -288,8 +285,8 @@
   </sheetPr>
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0" zoomScale="80" tabSelected="1">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0" zoomScale="80" tabSelected="1">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -302,7 +299,7 @@
     <col min="7" max="7" style="1" width="20.71304" bestFit="1" customWidth="1"/>
     <col min="8" max="8" style="1" width="20.32143" bestFit="1" customWidth="1"/>
     <col min="9" max="9" style="1" width="15.45408" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" style="1" width="17.69388" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" style="1" width="19.82024" bestFit="1" customWidth="1"/>
     <col min="11" max="11" style="1" width="118.5643" bestFit="1" customWidth="1"/>
     <col min="12" max="1025" style="1" width="14.51531" bestFit="1" customWidth="1"/>
     <col min="1026" max="16384" style="2"/>
@@ -428,17 +425,17 @@
         <v>Kill mod</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
+      <c r="G4" s="3" t="str">
+        <v>A15</v>
       </c>
       <c r="H4" s="3" t="str">
-        <v>ltch D0_control</v>
+        <v>D0_control</v>
       </c>
       <c r="I4" s="3" t="str">
         <v>ltch A19_ctrl</v>
       </c>
       <c r="J4" s="8" t="str">
-        <v>ltch_A19/SW1</v>
+        <v>ltch_A19/ltch_SW1</v>
       </c>
       <c r="K4" s="2" t="str">
         <v>Set A15 = '1' to ground it. Set D0_control = '1' to control D0. Vaue with "ltch" prefix will only be written if "Latch_en" is set in same command.</v>
@@ -477,7 +474,7 @@
     </row>
     <row r="6" spans="1:1025">
       <c r="A6" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>4</v>
@@ -512,7 +509,7 @@
     </row>
     <row r="7" spans="1:1025">
       <c r="A7" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
@@ -603,7 +600,7 @@
     </row>
     <row r="10" spans="1:1025">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
@@ -638,7 +635,7 @@
     </row>
     <row r="11" spans="1:1025">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
-Rework on LPC register map (last time I promise). -Added option to manually toggle a split bank even if booting from onboard flash (TSOP recovery case when TSOP is already split). -Work on IP keypad. -Dev menu to read GPI/O state -Moved TSOPcontrol enable bit from bit1 to bit0. -IP field will be limited to 0-255 and will be rediced to 255 if something higher is entered.
</commit_message>
<xml_diff>
--- a/XBlastMod register map.xlsx
+++ b/XBlastMod register map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14" count="14">
   <si>
     <t>Read</t>
   </si>
@@ -39,10 +39,13 @@
     <t>iSW2</t>
   </si>
   <si>
-    <t>iSW1/A19</t>
+    <t>iSW1</t>
   </si>
   <si>
     <t>Write</t>
+  </si>
+  <si>
+    <t>D0_control</t>
   </si>
   <si>
     <t>0xF701</t>
@@ -339,7 +342,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="80" tabSelected="1">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -351,7 +354,7 @@
     <col min="5" max="6" style="1" width="14.51531" bestFit="1" customWidth="1"/>
     <col min="7" max="7" style="1" width="20.71304" bestFit="1" customWidth="1"/>
     <col min="8" max="8" style="1" width="22.49865" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" style="1" width="19.82024" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" style="1" width="21.24872" bestFit="1" customWidth="1"/>
     <col min="10" max="10" style="1" width="13.74917" bestFit="1" customWidth="1"/>
     <col min="11" max="11" style="1" width="118.5643" bestFit="1" customWidth="1"/>
     <col min="12" max="1025" style="1" width="14.51531" bestFit="1" customWidth="1"/>
@@ -442,8 +445,8 @@
       <c r="E3" s="3" t="str">
         <v>A19ctrl</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>4</v>
+      <c r="F3" s="4" t="str">
+        <v>iSW1/A19</v>
       </c>
       <c r="G3" s="3" t="str">
         <v>#A19ctrl</v>
@@ -479,8 +482,8 @@
       <c r="G4" s="3" t="str">
         <v>A15</v>
       </c>
-      <c r="H4" s="12" t="str">
-        <v>D0_control</v>
+      <c r="H4" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="I4" s="3" t="str">
         <v>ltch_A19/ltch_SW1</v>
@@ -525,7 +528,7 @@
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>2</v>
@@ -560,7 +563,7 @@
     </row>
     <row r="7" spans="1:16384">
       <c r="A7" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>5</v>
@@ -628,16 +631,16 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3" t="str">
         <v>GPI-1</v>
@@ -646,10 +649,10 @@
         <v>GPI-0</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K9" s="16"/>
     </row>
@@ -666,10 +669,14 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="3" t="str">
+        <v>A19</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="I10" s="3" t="s">
         <v>4</v>
       </c>
@@ -688,22 +695,22 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K11" t="str">
         <v>GPO=General Purpose Output, GPO-2&amp;3 only accessed when SW1-2 = "11" &amp; D0_control = '1' &amp;A19ctrl = '0'</v>
@@ -727,9 +734,6 @@
     </row>
     <row r="18" spans="1:16384">
       <c r="G18" s="20"/>
-    </row>
-    <row r="21" spans="1:16384">
-      <c r="K21"/>
     </row>
     <row r="24" spans="1:16384">
       <c r="H24" s="20"/>

</xml_diff>